<commit_message>
Organizados arquivos em pastas e arquivos
</commit_message>
<xml_diff>
--- a/dados_temperatura_umidade.xlsx
+++ b/dados_temperatura_umidade.xlsx
@@ -408,10 +408,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>73%</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>73%</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>73%</t>
         </is>
       </c>
     </row>
@@ -642,37 +642,88 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="11" t="inlineStr">
+    <row r="14" ht="15" customHeight="1" s="7">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>26/04/2025 14:00:15</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
-        <is>
-          <t>25°</t>
-        </is>
-      </c>
-      <c r="C14" s="11" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="7">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>26/04/2025 14:00:31</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
-        <is>
-          <t>25°</t>
-        </is>
-      </c>
-      <c r="C15" s="11" t="inlineStr">
-        <is>
-          <t>67%</t>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="C15" s="10" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="7">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:24:18</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" s="7">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:25:16</t>
+        </is>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:30:08</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>65%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado gráfico de análise dados na planilha
</commit_message>
<xml_diff>
--- a/dados_temperatura_umidade.xlsx
+++ b/dados_temperatura_umidade.xlsx
@@ -408,7 +408,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
@@ -727,6 +727,57 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:53:14</t>
+        </is>
+      </c>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>26°</t>
+        </is>
+      </c>
+      <c r="C19" s="11" t="inlineStr">
+        <is>
+          <t>65%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:55:15</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>26°</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>65%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="inlineStr">
+        <is>
+          <t>26/04/2025 14:55:23</t>
+        </is>
+      </c>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>26°</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>65%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>